<commit_message>
fix error return java try catch
</commit_message>
<xml_diff>
--- a/web/uploads/data-unit_class (2) (2).xlsx
+++ b/web/uploads/data-unit_class (2) (2).xlsx
@@ -60,10 +60,10 @@
     <t>HOC_MOI</t>
   </si>
   <si>
-    <t>DHKTPM1ATT</t>
+    <t>DANG_CHO_SINH_VIEN_DANG_KY</t>
   </si>
   <si>
-    <t>DANG_CHO_SINH_VIEN_DANG_KY</t>
+    <t>DHKTPM1BTT</t>
   </si>
 </sst>
 </file>
@@ -109,11 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,8 +332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -381,7 +382,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3">
         <v>45079.708333333336</v>
@@ -401,11 +402,11 @@
       <c r="G2" s="1">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="J2" s="1">
         <v>315067680</v>

</xml_diff>